<commit_message>
add k-map for sum and c_out and fix full_adder module
</commit_message>
<xml_diff>
--- a/design_file/truth_table.xlsx
+++ b/design_file/truth_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Minh Đức\Đại học\Thiết kế vi mạch (TN)\miniproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_vivado\miniproject\design_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB695B-5162-4120-A666-E5B310F6D52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE17ED7-493C-49DE-99FE-6C87CF87B803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>a</t>
   </si>
@@ -59,6 +59,48 @@
   </si>
   <si>
     <t>=&gt; c_out = a AND b</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>K-map for sum</t>
+  </si>
+  <si>
+    <t>c_in ( c )</t>
+  </si>
+  <si>
+    <t>=&gt; sum = a'b'c + a'bc' + abc + ab'c'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=&gt; sum = a XOR b XOR c </t>
+  </si>
+  <si>
+    <t>K-map for c_out</t>
+  </si>
+  <si>
+    <t>=&gt; c_out = bc + ac + ab</t>
+  </si>
+  <si>
+    <t>=&gt; c_out = ab OR ac OR bc</t>
   </si>
 </sst>
 </file>
@@ -89,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -149,20 +191,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -173,19 +316,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -478,7 +666,7 @@
     <col min="1" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -487,176 +675,335 @@
       <c r="D1" s="6"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
+      <c r="I3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="P3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="16"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="22">
+        <v>1</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="21">
+        <v>0</v>
+      </c>
+      <c r="S6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="22">
+        <v>1</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0</v>
+      </c>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="22">
+        <v>0</v>
+      </c>
+      <c r="S7" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="22">
+        <v>0</v>
+      </c>
+      <c r="L8" s="22">
+        <v>1</v>
+      </c>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="22">
+        <v>1</v>
+      </c>
+      <c r="S8" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="22">
+        <v>1</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0</v>
+      </c>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="22">
+        <v>0</v>
+      </c>
+      <c r="S9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="P11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="13">
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="P6:P9"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -676,90 +1023,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
-        <v>0</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
-        <v>1</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -772,12 +1119,12 @@
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
add module full adder 8bit and check with golden model
</commit_message>
<xml_diff>
--- a/design_file/truth_table.xlsx
+++ b/design_file/truth_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code_vivado\miniproject\design_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE17ED7-493C-49DE-99FE-6C87CF87B803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644CC65B-78D9-470A-8E93-69084F8F887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,6 +306,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,62 +369,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="117" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -667,24 +667,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -702,18 +702,18 @@
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
-      <c r="P3" s="12" t="s">
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
+      <c r="P3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -731,18 +731,18 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="13" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="13" t="s">
+      <c r="L4" s="19"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="14"/>
+      <c r="S4" s="19"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
@@ -760,20 +760,20 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="19" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="19" t="s">
+      <c r="P5" s="12"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -793,28 +793,28 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="21">
-        <v>0</v>
-      </c>
-      <c r="L6" s="22">
-        <v>1</v>
-      </c>
-      <c r="P6" s="17" t="s">
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="21">
-        <v>0</v>
-      </c>
-      <c r="S6" s="22">
+      <c r="R6" s="7">
+        <v>0</v>
+      </c>
+      <c r="S6" s="8">
         <v>0</v>
       </c>
     </row>
@@ -834,24 +834,24 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="19" t="s">
+      <c r="I7" s="20"/>
+      <c r="J7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="22">
-        <v>1</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0</v>
-      </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="19" t="s">
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="22">
-        <v>0</v>
-      </c>
-      <c r="S7" s="22">
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7" s="8">
         <v>1</v>
       </c>
     </row>
@@ -871,24 +871,24 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="19" t="s">
+      <c r="I8" s="20"/>
+      <c r="J8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="22">
-        <v>0</v>
-      </c>
-      <c r="L8" s="22">
-        <v>1</v>
-      </c>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="19" t="s">
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="22">
-        <v>1</v>
-      </c>
-      <c r="S8" s="22">
+      <c r="R8" s="8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="8">
         <v>1</v>
       </c>
     </row>
@@ -908,24 +908,24 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="23" t="s">
+      <c r="I9" s="21"/>
+      <c r="J9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="22">
-        <v>1</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0</v>
-      </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="23" t="s">
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="22">
-        <v>0</v>
-      </c>
-      <c r="S9" s="22">
+      <c r="R9" s="8">
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
         <v>1</v>
       </c>
     </row>
@@ -962,35 +962,41 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="P11" s="9" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="P11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="P12" s="9" t="s">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="P12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="P3:S3"/>
@@ -998,12 +1004,6 @@
     <mergeCell ref="P6:P9"/>
     <mergeCell ref="P11:S11"/>
     <mergeCell ref="P12:S12"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="I3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1023,22 +1023,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1111,20 +1111,20 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>